<commit_message>
Code included earlier for test removed
</commit_message>
<xml_diff>
--- a/P&L Reports Generator/Backend/app/trial_balance.xlsx
+++ b/P&L Reports Generator/Backend/app/trial_balance.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CBDE1B3-36FA-49ED-9E7D-E07DD69584C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19890" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -135,76 +131,418 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -221,41 +559,327 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -304,7 +928,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -337,26 +961,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -389,23 +996,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,275 +1157,271 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="3" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="11.8583333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
+    <row r="1" ht="15" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="15" spans="1:1">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="14.25" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>25000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="14.25" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>45000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>75000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="14.25" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="14.25" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="14.25" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>120000</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+    <row r="9" ht="14.25" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
+    <row r="10" ht="15" spans="1:1">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+    <row r="11" ht="14.25" spans="1:3">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+    <row r="12" ht="14.25" spans="1:3">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>9000</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+    <row r="13" ht="14.25" spans="1:3">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>6000</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+    <row r="14" ht="14.25" spans="1:3">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>20000</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
+    <row r="15" ht="15" spans="1:1">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+    <row r="16" ht="14.25" spans="1:3">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1" t="s">
+    <row r="17" ht="14.25" spans="1:3">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1" t="s">
+    <row r="18" ht="14.25" spans="1:3">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>10000</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" ht="15" spans="1:1">
+      <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
+    <row r="20" ht="14.25" spans="1:3">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>300000</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="2" t="s">
+    <row r="21" ht="15" spans="1:1">
+      <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
+    <row r="22" ht="14.25" spans="1:2">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>180000</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
+    <row r="23" ht="14.25" spans="1:8">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>60000</v>
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
+    <row r="24" ht="14.25" spans="1:2">
+      <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>30000</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1" t="s">
+    <row r="25" ht="14.25" spans="1:2">
+      <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1" t="s">
+    <row r="26" ht="14.25" spans="1:2">
+      <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>10000</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1" t="s">
+    <row r="27" ht="14.25" spans="1:2">
+      <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>5000</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
+    <row r="28" ht="14.25" spans="1:3">
+      <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>2000</v>
       </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1" t="s">
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" ht="14.25" spans="1:2">
+      <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1" t="s">
+    <row r="30" ht="14.25" spans="1:3">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>2000</v>
       </c>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="2" t="s">
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" ht="15" spans="1:3">
+      <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="9">
         <f>SUM(B3:B30)</f>
         <v>580000</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="9">
         <f>SUM(C9:C30)</f>
         <v>580000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>